<commit_message>
Deployed fe1746dc with MkDocs version: 1.4.3
</commit_message>
<xml_diff>
--- a/assets/tables/furniture.xlsx
+++ b/assets/tables/furniture.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="179">
   <si>
     <t>Hero</t>
   </si>
@@ -58,7 +58,7 @@
     <t>HASTE</t>
   </si>
   <si>
-    <t>aTalene</t>
+    <t>Awk.Talene</t>
   </si>
   <si>
     <t>HR</t>
@@ -70,7 +70,7 @@
     <t>MP</t>
   </si>
   <si>
-    <t>Athelia</t>
+    <t>Athalia</t>
   </si>
   <si>
     <t>AS</t>
@@ -82,13 +82,13 @@
     <t>PP</t>
   </si>
   <si>
-    <t>Audrea</t>
+    <t>Audrae</t>
   </si>
   <si>
     <t>Flora</t>
   </si>
   <si>
-    <t>Healus</t>
+    <t>Haelus</t>
   </si>
   <si>
     <t>CDR</t>
@@ -100,163 +100,166 @@
     <t xml:space="preserve">MP </t>
   </si>
   <si>
+    <t>TY</t>
+  </si>
+  <si>
+    <t>CBR</t>
+  </si>
+  <si>
+    <t>Orthros</t>
+  </si>
+  <si>
+    <t>Talene</t>
+  </si>
+  <si>
+    <t>Titus</t>
+  </si>
+  <si>
+    <t>Twins</t>
+  </si>
+  <si>
+    <t>Wukong</t>
+  </si>
+  <si>
+    <t>Zaphrael</t>
+  </si>
+  <si>
+    <t>aEzizh</t>
+  </si>
+  <si>
+    <t>Ezizh</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>Framton</t>
+  </si>
+  <si>
+    <t>Khazard</t>
+  </si>
+  <si>
+    <t>DODGE</t>
+  </si>
+  <si>
+    <t>Leofric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP </t>
+  </si>
+  <si>
+    <t>Lucretia</t>
+  </si>
+  <si>
+    <t>Mehira</t>
+  </si>
+  <si>
+    <t>Mezoth</t>
+  </si>
+  <si>
+    <t>Mortas</t>
+  </si>
+  <si>
+    <t>Vyloris</t>
+  </si>
+  <si>
+    <t>Zikis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zolrath </t>
+  </si>
+  <si>
+    <t>Awk.Thane</t>
+  </si>
+  <si>
+    <t>Belinda</t>
+  </si>
+  <si>
+    <t>Eluard</t>
+  </si>
+  <si>
+    <t>Estrilda</t>
+  </si>
+  <si>
+    <t>Fawkes</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>Gwyneth</t>
+  </si>
+  <si>
+    <t>Hendrik</t>
+  </si>
+  <si>
+    <t>Lucius</t>
+  </si>
+  <si>
+    <t>Morrow</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Peggy</t>
+  </si>
+  <si>
+    <t>Rainie</t>
+  </si>
+  <si>
+    <t>Rigby</t>
+  </si>
+  <si>
+    <t>Rosaline</t>
+  </si>
+  <si>
+    <t>Rowan</t>
+  </si>
+  <si>
+    <t>Scarlet</t>
+  </si>
+  <si>
+    <t>Sonja</t>
+  </si>
+  <si>
+    <t>Thane</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Awk.Brutus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TN </t>
+  </si>
+  <si>
+    <t>Alaro</t>
+  </si>
+  <si>
+    <t>Anasta</t>
+  </si>
+  <si>
+    <t>Anoki</t>
+  </si>
+  <si>
+    <t>Antandra</t>
+  </si>
+  <si>
+    <t>Brutus</t>
+  </si>
+  <si>
+    <t>Drez</t>
+  </si>
+  <si>
+    <t>Granit</t>
+  </si>
+  <si>
     <t>TN</t>
   </si>
   <si>
-    <t>CBR</t>
-  </si>
-  <si>
-    <t>Orthros</t>
-  </si>
-  <si>
-    <t>Talene</t>
-  </si>
-  <si>
-    <t>Titus</t>
-  </si>
-  <si>
-    <t>Twins</t>
-  </si>
-  <si>
-    <t>Wukong</t>
-  </si>
-  <si>
-    <t>Zaphrael</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TN </t>
-  </si>
-  <si>
-    <t>aEzizh</t>
-  </si>
-  <si>
-    <t>Ezizh</t>
-  </si>
-  <si>
-    <t>RH</t>
-  </si>
-  <si>
-    <t>Framton</t>
-  </si>
-  <si>
-    <t>Khazard</t>
-  </si>
-  <si>
-    <t>DODGE</t>
-  </si>
-  <si>
-    <t>Leofric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP </t>
-  </si>
-  <si>
-    <t>Lucretia</t>
-  </si>
-  <si>
-    <t>Mehira</t>
-  </si>
-  <si>
-    <t>Mezoth</t>
-  </si>
-  <si>
-    <t>Mortas</t>
-  </si>
-  <si>
-    <t>Vyloris</t>
-  </si>
-  <si>
-    <t>Zikis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zolrath </t>
-  </si>
-  <si>
-    <t>aThane</t>
-  </si>
-  <si>
-    <t>Belinda</t>
-  </si>
-  <si>
-    <t>Eluard</t>
-  </si>
-  <si>
-    <t>Estrilda</t>
-  </si>
-  <si>
-    <t>Fawkes</t>
-  </si>
-  <si>
-    <t>LL</t>
-  </si>
-  <si>
-    <t>Gwyneth</t>
-  </si>
-  <si>
-    <t>Hendrik</t>
-  </si>
-  <si>
-    <t>Lucius</t>
-  </si>
-  <si>
-    <t>Morrow</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Peggy</t>
-  </si>
-  <si>
-    <t>Rainie</t>
-  </si>
-  <si>
-    <t>Rigby</t>
-  </si>
-  <si>
-    <t>Rosaline</t>
-  </si>
-  <si>
-    <t>Rowan</t>
-  </si>
-  <si>
-    <t>Scarlet</t>
-  </si>
-  <si>
-    <t>Sonja</t>
-  </si>
-  <si>
-    <t>Thane</t>
-  </si>
-  <si>
-    <t>Walker</t>
-  </si>
-  <si>
-    <t>aBrutus</t>
-  </si>
-  <si>
-    <t>Alaro</t>
-  </si>
-  <si>
-    <t>Anasta</t>
-  </si>
-  <si>
-    <t>Anoki</t>
-  </si>
-  <si>
-    <t>Antandra</t>
-  </si>
-  <si>
-    <t>Brutus</t>
-  </si>
-  <si>
-    <t>Drez</t>
-  </si>
-  <si>
-    <t>Granit</t>
-  </si>
-  <si>
-    <t>Khazos</t>
+    <t>Khasos</t>
   </si>
   <si>
     <t>Kren</t>
@@ -415,7 +418,7 @@
     <t>Ezio</t>
   </si>
   <si>
-    <t>JOA</t>
+    <t>Joan of Arc</t>
   </si>
   <si>
     <t>Joker</t>
@@ -475,7 +478,7 @@
     <t>LL - Life Leech</t>
   </si>
   <si>
-    <t>TN - Tenacity</t>
+    <t>TY - Tenacity</t>
   </si>
   <si>
     <t>PP- Physical Pierce</t>
@@ -555,7 +558,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,12 +576,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -665,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -673,7 +670,7 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -696,9 +693,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1011,13 +1005,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="31.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="27.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="27.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -1339,12 +1333,12 @@
         <v>13</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -1367,10 +1361,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>11</v>
@@ -1390,7 +1384,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>12</v>
@@ -1413,13 +1407,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
@@ -1431,12 +1425,12 @@
         <v>12</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
@@ -1445,7 +1439,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>11</v>
@@ -1459,7 +1453,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>8</v>
@@ -1468,7 +1462,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>8</v>
@@ -1482,7 +1476,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>25</v>
@@ -1505,7 +1499,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>11</v>
@@ -1528,7 +1522,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>8</v>
@@ -1537,7 +1531,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>8</v>
@@ -1551,7 +1545,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>20</v>
@@ -1574,7 +1568,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>12</v>
@@ -1583,7 +1577,7 @@
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>13</v>
@@ -1597,7 +1591,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>25</v>
@@ -1620,7 +1614,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
@@ -1643,7 +1637,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>20</v>
@@ -1666,7 +1660,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>12</v>
@@ -1675,10 +1669,10 @@
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>25</v>
@@ -1689,7 +1683,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>25</v>
@@ -1712,7 +1706,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>19</v>
@@ -1735,7 +1729,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>19</v>
@@ -1744,13 +1738,13 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>11</v>
@@ -1758,7 +1752,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>16</v>
@@ -1781,7 +1775,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>11</v>
@@ -1804,7 +1798,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
       <c r="A35" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>11</v>
@@ -1827,7 +1821,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>8</v>
@@ -1850,7 +1844,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>12</v>
@@ -1859,7 +1853,7 @@
         <v>25</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>12</v>
@@ -1873,7 +1867,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>15</v>
@@ -1896,7 +1890,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>20</v>
@@ -1905,7 +1899,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>15</v>
@@ -1919,10 +1913,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>11</v>
@@ -1942,7 +1936,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>11</v>
@@ -1951,7 +1945,7 @@
         <v>28</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>11</v>
@@ -1965,7 +1959,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
       <c r="A42" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>11</v>
@@ -1983,18 +1977,18 @@
         <v>12</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
       <c r="A43" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>13</v>
@@ -2011,7 +2005,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
       <c r="A44" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>8</v>
@@ -2034,7 +2028,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>19</v>
@@ -2057,7 +2051,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
       <c r="A46" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>16</v>
@@ -2066,13 +2060,13 @@
         <v>13</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>11</v>
@@ -2080,7 +2074,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
       <c r="A47" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>8</v>
@@ -2098,7 +2092,7 @@
         <v>11</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
@@ -2187,7 +2181,7 @@
         <v>10</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>8</v>
@@ -2204,7 +2198,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>21</v>
@@ -2221,13 +2215,13 @@
         <v>78</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>12</v>
@@ -2247,10 +2241,10 @@
         <v>11</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>11</v>
@@ -2264,7 +2258,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18">
       <c r="A55" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>25</v>
@@ -2279,15 +2273,15 @@
         <v>10</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18">
       <c r="A56" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>16</v>
@@ -2310,13 +2304,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
       <c r="A57" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>9</v>
@@ -2328,12 +2322,12 @@
         <v>15</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
       <c r="A58" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>19</v>
@@ -2356,7 +2350,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
       <c r="A59" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>25</v>
@@ -2365,13 +2359,13 @@
         <v>9</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>11</v>
@@ -2379,7 +2373,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
       <c r="A60" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>16</v>
@@ -2402,7 +2396,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
       <c r="A61" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>20</v>
@@ -2425,7 +2419,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
       <c r="A62" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>20</v>
@@ -2434,7 +2428,7 @@
         <v>9</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>11</v>
@@ -2443,18 +2437,18 @@
         <v>12</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
       <c r="A63" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>13</v>
@@ -2471,7 +2465,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
       <c r="A64" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>19</v>
@@ -2494,7 +2488,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
       <c r="A65" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>19</v>
@@ -2517,7 +2511,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
       <c r="A66" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>25</v>
@@ -2540,7 +2534,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
       <c r="A67" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>8</v>
@@ -2563,7 +2557,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
       <c r="A68" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>8</v>
@@ -2586,7 +2580,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
       <c r="A69" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>11</v>
@@ -2609,7 +2603,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18">
       <c r="A70" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>19</v>
@@ -2618,7 +2612,7 @@
         <v>9</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>10</v>
@@ -2632,7 +2626,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18">
       <c r="A71" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>8</v>
@@ -2655,7 +2649,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18">
       <c r="A72" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>19</v>
@@ -2678,7 +2672,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18">
       <c r="A73" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>11</v>
@@ -2687,7 +2681,7 @@
         <v>25</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>12</v>
@@ -2696,12 +2690,12 @@
         <v>13</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18">
       <c r="A74" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>8</v>
@@ -2713,7 +2707,7 @@
         <v>15</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>12</v>
@@ -2724,7 +2718,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
       <c r="A75" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>8</v>
@@ -2747,16 +2741,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
       <c r="A76" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>12</v>
@@ -2770,7 +2764,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
       <c r="A77" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>16</v>
@@ -2793,7 +2787,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
       <c r="A78" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>16</v>
@@ -2816,7 +2810,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
       <c r="A79" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>25</v>
@@ -2839,7 +2833,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
       <c r="A80" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>25</v>
@@ -2862,7 +2856,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
       <c r="A81" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>20</v>
@@ -2874,7 +2868,7 @@
         <v>13</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>12</v>
@@ -2885,7 +2879,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
       <c r="A82" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>8</v>
@@ -2903,12 +2897,12 @@
         <v>12</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
       <c r="A83" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>25</v>
@@ -2931,7 +2925,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
       <c r="A84" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>25</v>
@@ -2954,7 +2948,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
       <c r="A85" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>8</v>
@@ -2977,7 +2971,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18">
       <c r="A86" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>15</v>
@@ -2986,10 +2980,10 @@
         <v>8</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>12</v>
@@ -3000,7 +2994,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18">
       <c r="A87" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>8</v>
@@ -3012,7 +3006,7 @@
         <v>9</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>11</v>
@@ -3023,7 +3017,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18">
       <c r="A88" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>16</v>
@@ -3046,7 +3040,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18">
       <c r="A89" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>11</v>
@@ -3055,7 +3049,7 @@
         <v>8</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>21</v>
@@ -3069,7 +3063,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18">
       <c r="A90" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>11</v>
@@ -3078,7 +3072,7 @@
         <v>10</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>11</v>
@@ -3087,12 +3081,12 @@
         <v>13</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18">
       <c r="A91" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>20</v>
@@ -3110,15 +3104,15 @@
         <v>12</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18">
       <c r="A92" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>9</v>
@@ -3138,7 +3132,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18">
       <c r="A93" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>8</v>
@@ -3161,7 +3155,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18">
       <c r="A94" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>19</v>
@@ -3184,7 +3178,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18">
       <c r="A95" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>25</v>
@@ -3207,7 +3201,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18">
       <c r="A96" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>12</v>
@@ -3230,7 +3224,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18">
       <c r="A97" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>20</v>
@@ -3242,7 +3236,7 @@
         <v>25</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>12</v>
@@ -3253,10 +3247,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18">
       <c r="A98" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>11</v>
@@ -3276,7 +3270,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18">
       <c r="A99" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>16</v>
@@ -3299,7 +3293,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18">
       <c r="A100" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>11</v>
@@ -3308,7 +3302,7 @@
         <v>10</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>12</v>
@@ -3322,7 +3316,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18">
       <c r="A101" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>10</v>
@@ -3331,7 +3325,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>10</v>
@@ -3345,13 +3339,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18">
       <c r="A102" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>9</v>
@@ -3368,7 +3362,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18">
       <c r="A103" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>8</v>
@@ -3391,7 +3385,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18">
       <c r="A104" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>8</v>
@@ -3414,7 +3408,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18">
       <c r="A105" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>11</v>
@@ -3437,7 +3431,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18">
       <c r="A106" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>16</v>
@@ -3460,7 +3454,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18">
       <c r="A107" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>8</v>
@@ -3483,7 +3477,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18">
       <c r="A108" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>12</v>
@@ -3492,7 +3486,7 @@
         <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>12</v>
@@ -3506,7 +3500,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18">
       <c r="A109" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>8</v>
@@ -3529,7 +3523,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18">
       <c r="A110" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>8</v>
@@ -3552,16 +3546,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18">
       <c r="A111" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>11</v>
@@ -3575,7 +3569,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18">
       <c r="A112" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>19</v>
@@ -3598,7 +3592,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18">
       <c r="A113" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>16</v>
@@ -3613,7 +3607,7 @@
         <v>12</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>13</v>
@@ -3621,7 +3615,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18">
       <c r="A114" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>8</v>
@@ -3644,7 +3638,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18">
       <c r="A115" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>13</v>
@@ -3676,7 +3670,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18">
       <c r="A117" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -3686,66 +3680,66 @@
       <c r="G117" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18">
-      <c r="A118" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B118" s="11"/>
+      <c r="A118" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B118" s="3"/>
       <c r="C118" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18">
-      <c r="A119" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B119" s="11"/>
+      <c r="A119" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B119" s="3"/>
       <c r="C119" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18">
-      <c r="A120" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B120" s="11"/>
+      <c r="A120" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B120" s="3"/>
       <c r="C120" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18">
@@ -3754,16 +3748,16 @@
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G121" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18">
       <c r="A122" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -3774,58 +3768,58 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18">
       <c r="A123" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18">
       <c r="A124" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G124" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18">
-      <c r="A125" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
+      <c r="A125" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>